<commit_message>
add negative test cases scripe for Invoice and Reports module
</commit_message>
<xml_diff>
--- a/tests/artifact/data/Invoice.data.xlsx
+++ b/tests/artifact/data/Invoice.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="158">
   <si>
     <t>schema.path</t>
   </si>
@@ -485,6 +485,30 @@
   </si>
   <si>
     <t>For Profit</t>
+  </si>
+  <si>
+    <t>negative.inv</t>
+  </si>
+  <si>
+    <t>, ,%?,Gnukhata_id,@?$1,!@#$%.?,invalid,12str,v2.1,+</t>
+  </si>
+  <si>
+    <t>negative.type</t>
+  </si>
+  <si>
+    <t>, ,%?,Gnukhata_id,@?$1,!@#$%.?,invalid,12str,v2.1,-</t>
+  </si>
+  <si>
+    <t>calculateFrom</t>
+  </si>
+  <si>
+    <t>01-04-2022</t>
+  </si>
+  <si>
+    <t>calculateTo</t>
+  </si>
+  <si>
+    <t>31-03-2023</t>
   </si>
 </sst>
 </file>
@@ -1589,7 +1613,7 @@
   <dimension ref="A1:B116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A82" sqref="$A82:$XFD82"/>
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -2254,17 +2278,37 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A83" s="5"/>
-    </row>
-    <row r="84" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A84" s="5"/>
-    </row>
-    <row r="85" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A85" s="5"/>
-    </row>
-    <row r="86" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A86" s="5"/>
+    <row r="83" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A83" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="84" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A84" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="85" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A85" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A86" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="87" ht="23.1" customHeight="1" spans="1:1">
       <c r="A87" s="5"/>
@@ -2359,157 +2403,225 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0" objects="1"/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="beginsWith" dxfId="0" priority="15" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="0" priority="33" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A24,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="16" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="1" priority="34" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="17" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="2" priority="35" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="36" stopIfTrue="1">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="beginsWith" dxfId="0" priority="31" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="0" priority="49" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A25,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="32" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="1" priority="50" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="33" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="2" priority="51" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="34" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="52" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="beginsWith" dxfId="0" priority="37" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="0" priority="55" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A30,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="38" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="1" priority="56" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A30,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="39" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="2" priority="57" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A30,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="40" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="58" stopIfTrue="1">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="4" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="59" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="42">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="60">
       <formula>LEN(TRIM(B30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="12" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="30" stopIfTrue="1">
       <formula>LEN(TRIM(A81))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="11" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="2" priority="29" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A81,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="10" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="1" priority="28" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A81,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="9" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="0" priority="27" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A81,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81:E81">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="32">
       <formula>LEN(TRIM(B81))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="31" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="22" stopIfTrue="1">
       <formula>LEN(TRIM(A82))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="2" priority="21" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A82,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="1" priority="20" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A82,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="0" priority="19" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A82,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="24">
+      <formula>LEN(TRIM(B82))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="23" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:E82">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="26">
+      <formula>LEN(TRIM(C82))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="25" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="12">
+      <formula>LEN(TRIM(B83))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="11" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B84">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="10">
+      <formula>LEN(TRIM(B84))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:A23">
+    <cfRule type="beginsWith" dxfId="0" priority="43" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A20,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="44" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A20,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="45" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A20,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="46" stopIfTrue="1">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83:A84">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="16" stopIfTrue="1">
+      <formula>LEN(TRIM(A83))&gt;0</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="15" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A83,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="14" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A83,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="13" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A83,LEN("//"))="//"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85:A86">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A85))&gt;0</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A85,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A85,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A85,LEN("//"))="//"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:B23">
+    <cfRule type="expression" dxfId="4" priority="47" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="48">
+      <formula>LEN(TRIM(B20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:B25">
+    <cfRule type="expression" dxfId="4" priority="53" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="54">
+      <formula>LEN(TRIM(B24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B85:B86">
     <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(B82))&gt;0</formula>
+      <formula>LEN(TRIM(B85))&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:E82">
+  <conditionalFormatting sqref="A1:A19 A26:A29 A31:A80 A87:A1048576">
+    <cfRule type="beginsWith" dxfId="0" priority="61" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="62" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="63" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="64" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:E19 C20:E25 B26:E29 C30:E30 B31:E80 B87:E1048576">
+    <cfRule type="expression" dxfId="4" priority="65" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="68">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C83:E84">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="18">
+      <formula>LEN(TRIM(C83))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="17" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C85:E86">
     <cfRule type="notContainsBlanks" dxfId="5" priority="8">
-      <formula>LEN(TRIM(C82))&gt;0</formula>
+      <formula>LEN(TRIM(C85))&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20:A23">
-    <cfRule type="beginsWith" dxfId="0" priority="25" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A20,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="26" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A20,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="27" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A20,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="28" stopIfTrue="1">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20:B23">
-    <cfRule type="expression" dxfId="4" priority="29" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="30">
-      <formula>LEN(TRIM(B20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:B25">
-    <cfRule type="expression" dxfId="4" priority="35" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="36">
-      <formula>LEN(TRIM(B24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A19 A26:A29 A31:A80 A83:A1048576">
-    <cfRule type="beginsWith" dxfId="0" priority="43" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="44" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="45" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="46" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E19 C20:E25 B26:E29 C30:E30 B31:E80 B83:E1048576">
-    <cfRule type="expression" dxfId="4" priority="47" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="50">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>